<commit_message>
fix parse input 2
</commit_message>
<xml_diff>
--- a/pythonProject/input/Input modello sessione invernale.xlsx
+++ b/pythonProject/input/Input modello sessione invernale.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Input generali" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="136">
   <si>
     <t>Aule disponibili</t>
   </si>
@@ -638,6 +638,9 @@
   <si>
     <t>Aula B, Aula C</t>
   </si>
+  <si>
+    <t>Aula A, Aula B, Aula C,Aula D</t>
+  </si>
 </sst>
 </file>
 
@@ -1146,7 +1149,7 @@
   <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1220,15 +1223,11 @@
       <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="5">
-        <v>44965</v>
-      </c>
+      <c r="F3" s="5"/>
       <c r="H3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="5">
-        <v>44965</v>
-      </c>
+      <c r="I3" s="5"/>
       <c r="K3" s="6" t="s">
         <v>13</v>
       </c>
@@ -1243,15 +1242,11 @@
       <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="5">
-        <v>44965</v>
-      </c>
+      <c r="F4" s="5"/>
       <c r="H4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="5">
-        <v>44965</v>
-      </c>
+      <c r="I4" s="5"/>
       <c r="K4" s="6" t="s">
         <v>16</v>
       </c>
@@ -1266,15 +1261,11 @@
       <c r="E5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="5">
-        <v>44965</v>
-      </c>
+      <c r="F5" s="5"/>
       <c r="H5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="5">
-        <v>44965</v>
-      </c>
+      <c r="I5" s="5"/>
       <c r="K5" s="6" t="s">
         <v>19</v>
       </c>
@@ -1289,15 +1280,11 @@
       <c r="E6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="5">
-        <v>44965</v>
-      </c>
+      <c r="F6" s="5"/>
       <c r="H6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="5">
-        <v>44965</v>
-      </c>
+      <c r="I6" s="5"/>
       <c r="K6" s="6" t="s">
         <v>22</v>
       </c>
@@ -1312,15 +1299,11 @@
       <c r="E7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="5">
-        <v>44965</v>
-      </c>
+      <c r="F7" s="5"/>
       <c r="H7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="5">
-        <v>44965</v>
-      </c>
+      <c r="I7" s="5"/>
       <c r="K7" s="10" t="s">
         <v>25</v>
       </c>
@@ -1333,9 +1316,7 @@
       <c r="E8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="5">
-        <v>44965</v>
-      </c>
+      <c r="F8" s="5"/>
       <c r="H8" s="4"/>
       <c r="I8" s="5"/>
       <c r="K8" s="10" t="s">
@@ -1349,9 +1330,7 @@
       <c r="E9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="5">
-        <v>44965</v>
-      </c>
+      <c r="F9" s="5"/>
       <c r="H9" s="4"/>
       <c r="I9" s="5"/>
       <c r="K9" s="10" t="s">
@@ -1365,9 +1344,7 @@
       <c r="E10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="5">
-        <v>44965</v>
-      </c>
+      <c r="F10" s="5"/>
       <c r="H10" s="4"/>
       <c r="I10" s="5"/>
       <c r="K10" s="10"/>
@@ -4373,7 +4350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -20377,7 +20354,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -20469,7 +20448,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="G2" s="16">
         <v>1</v>

</xml_diff>

<commit_message>
Aggiunta modelli con indisponibilità
</commit_message>
<xml_diff>
--- a/pythonProject/input/Input modello sessione invernale.xlsx
+++ b/pythonProject/input/Input modello sessione invernale.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Input generali" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="140">
   <si>
     <t xml:space="preserve">Aule disponibili</t>
   </si>
@@ -88,16 +88,10 @@
     <t xml:space="preserve">Aula D</t>
   </si>
   <si>
-    <t xml:space="preserve">Laboratorio Babbage</t>
-  </si>
-  <si>
     <t xml:space="preserve">Guadagno giorni preferiti</t>
   </si>
   <si>
     <t xml:space="preserve">Aula E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laboratorio Postel</t>
   </si>
   <si>
     <t xml:space="preserve">Importanza primo anno</t>
@@ -115,7 +109,7 @@
     <t xml:space="preserve">Importanza terzo anno</t>
   </si>
   <si>
-    <t xml:space="preserve">Aula G</t>
+    <t xml:space="preserve">Importanza distanza esami</t>
   </si>
   <si>
     <t xml:space="preserve">Nome corso</t>
@@ -996,25 +990,21 @@
   </sheetPr>
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="39.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="27.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="13" style="0" width="12.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1129,12 +1119,10 @@
         <v>20</v>
       </c>
       <c r="F6" s="6"/>
-      <c r="H6" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="H6" s="5"/>
       <c r="I6" s="6"/>
       <c r="K6" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L6" s="8" t="n">
         <v>2</v>
@@ -1145,15 +1133,13 @@
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="E7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="6"/>
-      <c r="H7" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="H7" s="5"/>
       <c r="I7" s="6"/>
       <c r="K7" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L7" s="12" t="n">
         <v>10</v>
@@ -1162,13 +1148,13 @@
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C8" s="10"/>
       <c r="E8" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F8" s="6"/>
       <c r="H8" s="5"/>
       <c r="I8" s="6"/>
       <c r="K8" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L8" s="12" t="n">
         <v>4</v>
@@ -1176,27 +1162,29 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E9" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F9" s="6"/>
       <c r="H9" s="5"/>
       <c r="I9" s="6"/>
       <c r="K9" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L9" s="12" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E10" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="E10" s="5"/>
       <c r="F10" s="6"/>
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="12"/>
+      <c r="K10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="12" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E11" s="5"/>
@@ -4210,7 +4198,7 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="35.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.45"/>
@@ -4221,43 +4209,42 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="36.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="39.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="45.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="12" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="115.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="F1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="G1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="I1" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>39</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>41</v>
       </c>
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
@@ -4279,13 +4266,13 @@
     </row>
     <row r="2" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>44</v>
       </c>
       <c r="D2" s="18" t="n">
         <v>1</v>
@@ -4294,10 +4281,10 @@
         <v>2</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H2" s="18" t="n">
         <v>1</v>
@@ -4325,13 +4312,13 @@
     </row>
     <row r="3" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>47</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>49</v>
       </c>
       <c r="D3" s="18" t="n">
         <v>1</v>
@@ -4340,10 +4327,10 @@
         <v>2</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H3" s="18" t="n">
         <v>1</v>
@@ -4371,13 +4358,13 @@
     </row>
     <row r="4" customFormat="false" ht="60.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D4" s="18" t="n">
         <v>1</v>
@@ -4386,10 +4373,10 @@
         <v>2</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H4" s="18" t="n">
         <v>1</v>
@@ -4417,13 +4404,13 @@
     </row>
     <row r="5" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D5" s="18" t="n">
         <v>1</v>
@@ -4432,10 +4419,10 @@
         <v>2</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H5" s="18" t="n">
         <v>1</v>
@@ -4463,13 +4450,13 @@
     </row>
     <row r="6" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D6" s="18" t="n">
         <v>2</v>
@@ -4478,10 +4465,10 @@
         <v>2</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H6" s="18" t="n">
         <v>2</v>
@@ -4509,13 +4496,13 @@
     </row>
     <row r="7" customFormat="false" ht="62.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D7" s="18" t="n">
         <v>2</v>
@@ -4524,10 +4511,10 @@
         <v>2</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H7" s="18" t="n">
         <v>1</v>
@@ -4555,13 +4542,13 @@
     </row>
     <row r="8" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D8" s="18" t="n">
         <v>2</v>
@@ -4570,10 +4557,10 @@
         <v>2</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H8" s="18" t="n">
         <v>2</v>
@@ -4601,13 +4588,13 @@
     </row>
     <row r="9" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>64</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>66</v>
       </c>
       <c r="D9" s="18" t="n">
         <v>1.2</v>
@@ -4616,10 +4603,10 @@
         <v>2</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H9" s="18" t="n">
         <v>1</v>
@@ -11777,7 +11764,7 @@
       <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="35.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.45"/>
@@ -11788,43 +11775,42 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="36.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="39.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="45.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="12" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>39</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>41</v>
       </c>
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
@@ -11846,13 +11832,13 @@
     </row>
     <row r="2" customFormat="false" ht="51.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D2" s="18" t="n">
         <v>1</v>
@@ -11861,10 +11847,10 @@
         <v>2</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H2" s="18" t="n">
         <v>1</v>
@@ -11892,13 +11878,13 @@
     </row>
     <row r="3" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>71</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>73</v>
       </c>
       <c r="D3" s="18" t="n">
         <v>1</v>
@@ -11907,10 +11893,10 @@
         <v>2</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H3" s="18" t="n">
         <v>1</v>
@@ -11938,13 +11924,13 @@
     </row>
     <row r="4" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>75</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>77</v>
       </c>
       <c r="D4" s="18" t="n">
         <v>1</v>
@@ -11953,10 +11939,10 @@
         <v>2</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H4" s="18" t="n">
         <v>1</v>
@@ -11984,13 +11970,13 @@
     </row>
     <row r="5" customFormat="false" ht="83.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>80</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>82</v>
       </c>
       <c r="D5" s="18" t="n">
         <v>2</v>
@@ -11999,10 +11985,10 @@
         <v>2</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H5" s="18" t="n">
         <v>1</v>
@@ -12030,13 +12016,13 @@
     </row>
     <row r="6" customFormat="false" ht="177" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>83</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>85</v>
       </c>
       <c r="D6" s="18" t="n">
         <v>2</v>
@@ -12045,10 +12031,10 @@
         <v>2</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H6" s="18" t="n">
         <v>1</v>
@@ -12076,13 +12062,13 @@
     </row>
     <row r="7" customFormat="false" ht="129" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>86</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>88</v>
       </c>
       <c r="D7" s="18" t="n">
         <v>2</v>
@@ -12091,10 +12077,10 @@
         <v>2</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H7" s="18" t="n">
         <v>1</v>
@@ -12122,13 +12108,13 @@
     </row>
     <row r="8" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>90</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>92</v>
       </c>
       <c r="D8" s="18" t="n">
         <v>2</v>
@@ -12137,10 +12123,10 @@
         <v>2</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H8" s="18" t="n">
         <v>1</v>
@@ -12168,13 +12154,13 @@
     </row>
     <row r="9" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>94</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>96</v>
       </c>
       <c r="D9" s="18" t="n">
         <v>2</v>
@@ -12183,10 +12169,10 @@
         <v>2</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H9" s="18" t="n">
         <v>1</v>
@@ -19340,11 +19326,11 @@
   </sheetPr>
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="35.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.45"/>
@@ -19355,43 +19341,42 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="36.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="39.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="45.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="12" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="67.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="16" t="s">
+      <c r="G1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="I1" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>39</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>41</v>
       </c>
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
@@ -19413,13 +19398,13 @@
     </row>
     <row r="2" customFormat="false" ht="88.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>98</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>100</v>
       </c>
       <c r="D2" s="18" t="n">
         <v>1</v>
@@ -19428,10 +19413,10 @@
         <v>2</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H2" s="18" t="n">
         <v>1</v>
@@ -19459,13 +19444,13 @@
     </row>
     <row r="3" customFormat="false" ht="88.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>101</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>103</v>
       </c>
       <c r="D3" s="18" t="n">
         <v>1</v>
@@ -19474,10 +19459,10 @@
         <v>2</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H3" s="18" t="n">
         <v>1</v>
@@ -19505,13 +19490,13 @@
     </row>
     <row r="4" customFormat="false" ht="88.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D4" s="18" t="n">
         <v>1</v>
@@ -19520,10 +19505,10 @@
         <v>2</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H4" s="18" t="n">
         <v>1</v>
@@ -19551,13 +19536,13 @@
     </row>
     <row r="5" customFormat="false" ht="51.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>106</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>108</v>
       </c>
       <c r="D5" s="18" t="n">
         <v>1</v>
@@ -19566,10 +19551,10 @@
         <v>2</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H5" s="18" t="n">
         <v>1</v>
@@ -19597,13 +19582,13 @@
     </row>
     <row r="6" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D6" s="18" t="n">
         <v>1</v>
@@ -19612,10 +19597,10 @@
         <v>2</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H6" s="18" t="n">
         <v>1</v>
@@ -19643,13 +19628,13 @@
     </row>
     <row r="7" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D7" s="18" t="n">
         <v>1</v>
@@ -19658,10 +19643,10 @@
         <v>2</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H7" s="18" t="n">
         <v>1</v>
@@ -19689,13 +19674,13 @@
     </row>
     <row r="8" customFormat="false" ht="62.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D8" s="18" t="n">
         <v>1</v>
@@ -19704,10 +19689,10 @@
         <v>2</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H8" s="18" t="n">
         <v>1</v>
@@ -19735,13 +19720,13 @@
     </row>
     <row r="9" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>117</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>119</v>
       </c>
       <c r="D9" s="18" t="n">
         <v>1</v>
@@ -19750,10 +19735,10 @@
         <v>2</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H9" s="18" t="n">
         <v>1</v>
@@ -19781,13 +19766,13 @@
     </row>
     <row r="10" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="18" t="s">
         <v>121</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>123</v>
       </c>
       <c r="D10" s="18" t="n">
         <v>1</v>
@@ -19796,10 +19781,10 @@
         <v>2</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H10" s="18" t="n">
         <v>1</v>
@@ -19827,13 +19812,13 @@
     </row>
     <row r="11" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D11" s="18" t="n">
         <v>1.2</v>
@@ -19842,10 +19827,10 @@
         <v>2</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H11" s="18" t="n">
         <v>1</v>
@@ -19873,13 +19858,13 @@
     </row>
     <row r="12" customFormat="false" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D12" s="18" t="n">
         <v>2</v>
@@ -19888,10 +19873,10 @@
         <v>2</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H12" s="18" t="n">
         <v>1</v>
@@ -19919,13 +19904,13 @@
     </row>
     <row r="13" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D13" s="18" t="n">
         <v>2</v>
@@ -19934,10 +19919,10 @@
         <v>2</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H13" s="18" t="n">
         <v>1</v>
@@ -19965,13 +19950,13 @@
     </row>
     <row r="14" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" s="18" t="s">
         <v>130</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>132</v>
       </c>
       <c r="D14" s="18" t="n">
         <v>2</v>
@@ -19980,10 +19965,10 @@
         <v>2</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H14" s="18" t="n">
         <v>1</v>
@@ -20011,13 +19996,13 @@
     </row>
     <row r="15" customFormat="false" ht="53.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" s="18" t="s">
         <v>134</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>136</v>
       </c>
       <c r="D15" s="18" t="n">
         <v>1.2</v>
@@ -20026,10 +20011,10 @@
         <v>2</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H15" s="18" t="n">
         <v>1</v>
@@ -20057,13 +20042,13 @@
     </row>
     <row r="16" customFormat="false" ht="60.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D16" s="18" t="n">
         <v>1.2</v>
@@ -20072,10 +20057,10 @@
         <v>2</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H16" s="18" t="n">
         <v>1</v>
@@ -20103,13 +20088,13 @@
     </row>
     <row r="17" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D17" s="18" t="n">
         <v>1.2</v>
@@ -20118,10 +20103,10 @@
         <v>2</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H17" s="18" t="n">
         <v>1</v>

</xml_diff>